<commit_message>
some changes with my login validation
</commit_message>
<xml_diff>
--- a/database/clexan_foods.xlsx
+++ b/database/clexan_foods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Clarkstore\worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Clarkstore\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD5901E3-B517-4D4E-BFBA-3497730DC525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A394142-764E-42B7-A8F2-8BCC44BE2D96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{334EE45C-64B1-45AE-96E3-202C83F441C2}"/>
   </bookViews>
@@ -305,14 +305,11 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color theme="9"/>
         </left>
-        <right style="medium">
-          <color theme="9"/>
-        </right>
+        <right/>
         <top style="medium">
           <color theme="9"/>
         </top>
@@ -324,11 +321,14 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color theme="9"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color theme="9"/>
+        </right>
         <top style="medium">
           <color theme="9"/>
         </top>
@@ -475,8 +475,8 @@
     <tableColumn id="1" xr3:uid="{89DCBA5C-0E54-456D-93BF-963D37219245}" uniqueName="1" name="itemID" queryTableFieldId="1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{6732FB10-7307-4104-93D3-576BD157C746}" uniqueName="2" name="item_name" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{FE6016A6-1F1C-4891-B496-01B50A324816}" uniqueName="3" name="item_type" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B5BB543F-B2D0-4D7D-A1AB-C05C9BE38BF6}" uniqueName="4" name="unit_price" queryTableFieldId="4" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{2D6B141F-78FB-48FE-B972-AA905846EE15}" uniqueName="5" name="in_stock" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B5BB543F-B2D0-4D7D-A1AB-C05C9BE38BF6}" uniqueName="4" name="unit_price" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2D6B141F-78FB-48FE-B972-AA905846EE15}" uniqueName="5" name="in_stock" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>